<commit_message>
Qual flow updated, Increaed the App launch delay time to 20 seconds from 10.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/QualProcessTestData.xlsx
+++ b/src/test/resources/TestData/QualProcessTestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SSC\git\VRT\src\test\resources\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manoj.ghadei\git\VRT\QualFlowVRT\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7AA14F6-A03F-45C6-835D-BBF772F598EB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E184BFB-5D97-4DDC-A272-EFC868BED480}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="11070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="QUAL001" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
   <si>
     <t>UID</t>
   </si>
@@ -73,13 +73,16 @@
   </si>
   <si>
     <t>A-Asset-Test2</t>
+  </si>
+  <si>
+    <t>RunNo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -89,6 +92,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -135,16 +146,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -426,101 +440,112 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="22.68359375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.68359375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.7890625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.7890625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.41796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="4"/>
+    <col min="5" max="5" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="1" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
QualFlowVRT updated with the below changes: -	Missing mapping alert message in Program loggers handled. -	Log files getting copied to the corresponding Study file instance folder in Documents folder.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/QualProcessTestData.xlsx
+++ b/src/test/resources/TestData/QualProcessTestData.xlsx
@@ -1,31 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manoj.ghadei\git\VRT\QualFlowVRT\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E184BFB-5D97-4DDC-A272-EFC868BED480}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC450381-14AD-40A5-B1C3-81F661FDD20B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="11070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="QUAL001" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+  <si>
+    <t>RunNo</t>
+  </si>
   <si>
     <t>UID</t>
   </si>
@@ -33,49 +36,55 @@
     <t>PW</t>
   </si>
   <si>
+    <t>Aname</t>
+  </si>
+  <si>
+    <t>Sname</t>
+  </si>
+  <si>
+    <t>BSIP</t>
+  </si>
+  <si>
+    <t>SetupSOP</t>
+  </si>
+  <si>
+    <t>StudyTimeInMinutes</t>
+  </si>
+  <si>
+    <t>StudySaveComment</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Asset01</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
     <t>1</t>
   </si>
   <si>
-    <t>Aname</t>
-  </si>
-  <si>
-    <t>Sname</t>
-  </si>
-  <si>
-    <t>BSIP</t>
-  </si>
-  <si>
-    <t>SetupSOP</t>
-  </si>
-  <si>
-    <t>Test1</t>
-  </si>
-  <si>
-    <t>StudyTimeInMinutes</t>
-  </si>
-  <si>
-    <t>StudySaveComment</t>
-  </si>
-  <si>
     <t>111111</t>
   </si>
   <si>
-    <t>A-Asset-Test1</t>
-  </si>
-  <si>
-    <t>Asset01</t>
-  </si>
-  <si>
-    <t>setup-1</t>
-  </si>
-  <si>
-    <t>10.17.18.61</t>
-  </si>
-  <si>
-    <t>A-Asset-Test2</t>
-  </si>
-  <si>
-    <t>RunNo</t>
+    <t>10.17.18.109</t>
+  </si>
+  <si>
+    <t>Test2</t>
+  </si>
+  <si>
+    <t>qualstart-2</t>
+  </si>
+  <si>
+    <t>Test3</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>qualstart-3</t>
   </si>
 </sst>
 </file>
@@ -85,24 +94,24 @@
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -115,7 +124,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -129,16 +138,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -148,16 +157,16 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -194,7 +203,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -206,7 +215,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -253,6 +262,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -288,6 +314,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -442,29 +485,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="4"/>
-    <col min="5" max="5" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>3</v>
@@ -479,73 +522,73 @@
         <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="B2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="E2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>11</v>
+      <c r="G2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="B3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="E3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>15</v>
+      <c r="G3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Comitting the updated code of qualflow to git
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/QualProcessTestData.xlsx
+++ b/src/test/resources/TestData/QualProcessTestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manoj.ghadei\git\VRT\QualFlowVRT\src\test\resources\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ruchika.Behura\git\QualFlowVRT\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC450381-14AD-40A5-B1C3-81F661FDD20B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BE7020F-07B0-4C86-BF37-74B3A0A30AF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="135" yWindow="135" windowWidth="20355" windowHeight="10785" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="QUAL001" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>RunNo</t>
   </si>
@@ -54,37 +54,28 @@
     <t>StudySaveComment</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>Asset01</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
-    <t>111111</t>
-  </si>
-  <si>
-    <t>10.17.18.109</t>
-  </si>
-  <si>
-    <t>Test2</t>
-  </si>
-  <si>
-    <t>qualstart-2</t>
-  </si>
-  <si>
-    <t>Test3</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>qualstart-3</t>
+    <t>Test1</t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>123456</t>
+  </si>
+  <si>
+    <t>10.17.18.88</t>
+  </si>
+  <si>
+    <t>Setup-1</t>
+  </si>
+  <si>
+    <t>Ast1</t>
+  </si>
+  <si>
+    <t>7</t>
   </si>
 </sst>
 </file>
@@ -163,10 +154,10 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -483,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -530,60 +521,31 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="H2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>